<commit_message>
fixed up some figures/tables
</commit_message>
<xml_diff>
--- a/analyses/productivity/tables/TableS1_stock_key.xlsx
+++ b/analyses/productivity/tables/TableS1_stock_key.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/wc_cc_synthesis/analyses/productivity/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5321D7C-5ACC-2849-A380-5F3991F55E88}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{757C523C-BCAA-1545-B95A-379FA219E039}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16600" yWindow="5760" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12380" yWindow="500" windowWidth="33720" windowHeight="26360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="TableS1_stock_key" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="270">
   <si>
     <t>Canada West Coast</t>
   </si>
@@ -28,516 +28,261 @@
     <t>BOCACCBCW</t>
   </si>
   <si>
-    <t>Bocaccio British Columbia Waters</t>
-  </si>
-  <si>
     <t>CROCKWCVANISOGQCI</t>
   </si>
   <si>
-    <t>Canary rockfish West Coast of Vancouver Island and Strait of Georgia and Queen Charlotte Islands</t>
-  </si>
-  <si>
     <t>ESOLEHS</t>
   </si>
   <si>
-    <t>English sole Hecate Strait</t>
-  </si>
-  <si>
     <t>HERRCC</t>
   </si>
   <si>
-    <t>Pacific herring Central Coast</t>
-  </si>
-  <si>
     <t>HERRPRD</t>
   </si>
   <si>
-    <t>Pacific herring Prince Rupert District</t>
-  </si>
-  <si>
     <t>HERRQCI</t>
   </si>
   <si>
-    <t>Pacific herring Queen Charlotte Islands</t>
-  </si>
-  <si>
     <t>HERRWCVANI</t>
   </si>
   <si>
-    <t>Pacific herring West Coast of Vancouver Island</t>
-  </si>
-  <si>
     <t>PCOD5AB</t>
   </si>
   <si>
-    <t>Pacific cod Queen Charlotte Sound</t>
-  </si>
-  <si>
     <t>PCODHS</t>
   </si>
   <si>
-    <t>Pacific cod Hecate Strait</t>
-  </si>
-  <si>
     <t>PCODWCVANI</t>
   </si>
   <si>
-    <t>Pacific cod West Coast of Vancouver Island</t>
-  </si>
-  <si>
     <t>PERCHQCI</t>
   </si>
   <si>
-    <t>Pacific ocean perch Haida Gwaii</t>
-  </si>
-  <si>
     <t>PERCHWCVANI</t>
   </si>
   <si>
-    <t>Pacific ocean perch West Coast of Vancouver Island</t>
-  </si>
-  <si>
     <t>RSOLE5AB</t>
   </si>
   <si>
-    <t>Rock sole Queen Charlotte Sound</t>
-  </si>
-  <si>
     <t>RSOLEHSTR</t>
   </si>
   <si>
-    <t>Rock sole Hecate Strait</t>
-  </si>
-  <si>
     <t>SABLEFPCAN</t>
   </si>
   <si>
-    <t>Sablefish Pacific Coast of Canada</t>
-  </si>
-  <si>
     <t>US Alaska</t>
   </si>
   <si>
     <t>ALPLAICBSAI</t>
   </si>
   <si>
-    <t>Alaska plaice Bering Sea and Aleutian Islands</t>
-  </si>
-  <si>
     <t>ARFLOUNDBSAI</t>
   </si>
   <si>
-    <t>Arrowtooth flounder Bering Sea and Aleutian Islands</t>
-  </si>
-  <si>
     <t>ARFLOUNDGA</t>
   </si>
   <si>
-    <t>Arrowtooth flounder Gulf of Alaska</t>
-  </si>
-  <si>
     <t>ATKABSAI</t>
   </si>
   <si>
-    <t>Atka mackerel Bering Sea and Aleutian Islands</t>
-  </si>
-  <si>
     <t>BKINGCRABPI</t>
   </si>
   <si>
-    <t>Blue king crab Pribilof Islands</t>
-  </si>
-  <si>
     <t>BKINGCRABSMI</t>
   </si>
   <si>
-    <t>Blue king crab Saint Matthews Island</t>
-  </si>
-  <si>
     <t>DSOLEGA</t>
   </si>
   <si>
-    <t>Dover sole Gulf of Alaska</t>
-  </si>
-  <si>
     <t>DUSROCKGA</t>
   </si>
   <si>
-    <t>Dusky rockfish Gulf of Alaska</t>
-  </si>
-  <si>
     <t>FLSOLEBSAI</t>
   </si>
   <si>
-    <t>Flathead sole Bering Sea and Aleutian Islands</t>
-  </si>
-  <si>
     <t>FLSOLEGA</t>
   </si>
   <si>
-    <t>Flathead sole Gulf of Alaska</t>
-  </si>
-  <si>
     <t>GHALBSAI</t>
   </si>
   <si>
-    <t>Greenland halibut Bering Sea and Aleutian Islands</t>
-  </si>
-  <si>
     <t>HERRPWS</t>
   </si>
   <si>
-    <t>Pacific herring Prince William Sound</t>
-  </si>
-  <si>
     <t>HERRTOG</t>
   </si>
   <si>
-    <t>Pacific herring Togiak District</t>
-  </si>
-  <si>
     <t>NROCKBSAI</t>
   </si>
   <si>
-    <t>Northern rockfish Bering Sea and Aleutian Islands</t>
-  </si>
-  <si>
     <t>NROCKGA</t>
   </si>
   <si>
-    <t>Northern rockfish Gulf of Alaska</t>
-  </si>
-  <si>
     <t>NRSOLEEBSAI</t>
   </si>
   <si>
-    <t>Northern rock sole Eastern Bering Sea and Aleutian Islands</t>
-  </si>
-  <si>
     <t>PCODGA</t>
   </si>
   <si>
-    <t>Pacific cod Gulf of Alaska</t>
-  </si>
-  <si>
     <t>PERCHEBSAI</t>
   </si>
   <si>
-    <t>Pacific ocean perch Eastern Bering Sea and Aleutian Islands</t>
-  </si>
-  <si>
     <t>POPERCHGA</t>
   </si>
   <si>
-    <t>Pacific ocean perch Gulf of Alaska</t>
-  </si>
-  <si>
     <t>REXSOLEGA</t>
   </si>
   <si>
-    <t>Rex sole Gulf of Alaska</t>
-  </si>
-  <si>
     <t>REYEROCKBSAI</t>
   </si>
   <si>
-    <t>Rougheye rockfish Bering Sea and Aleutian Islands</t>
-  </si>
-  <si>
     <t>REYEROCKGA</t>
   </si>
   <si>
-    <t>Rougheye rockfish Gulf of Alaska</t>
-  </si>
-  <si>
     <t>RKCRABBB</t>
   </si>
   <si>
-    <t>Red king crab Bristol Bay</t>
-  </si>
-  <si>
     <t>RKCRABNS</t>
   </si>
   <si>
-    <t>Red king crab Norton Sound</t>
-  </si>
-  <si>
     <t>RKCRABPI</t>
   </si>
   <si>
-    <t>Red king crab Pribilof Islands</t>
-  </si>
-  <si>
     <t>SABLEFEBSAIGA</t>
   </si>
   <si>
-    <t>Sablefish Eastern Bering Sea / Aleutian Islands / Gulf of Alaska</t>
-  </si>
-  <si>
     <t>SNOWCRABBS</t>
   </si>
   <si>
-    <t>Snow crab Bering Sea</t>
-  </si>
-  <si>
     <t>TANNERCRABBSAI</t>
   </si>
   <si>
-    <t>Tanner crab Bering Sea and Aleutian Islands</t>
-  </si>
-  <si>
     <t>WPOLLAI</t>
   </si>
   <si>
-    <t>Walleye pollock Aleutian Islands</t>
-  </si>
-  <si>
     <t>WPOLLEBS</t>
   </si>
   <si>
-    <t>Walleye pollock Eastern Bering Sea</t>
-  </si>
-  <si>
     <t>WPOLLGA</t>
   </si>
   <si>
-    <t>Walleye pollock Gulf of Alaska</t>
-  </si>
-  <si>
     <t>YSOLEBSAI</t>
   </si>
   <si>
-    <t>Yellowfin sole Bering Sea and Aleutian Islands</t>
-  </si>
-  <si>
     <t>US West Coast</t>
   </si>
   <si>
     <t>ARFLOUNDPCOAST</t>
   </si>
   <si>
-    <t>Arrowtooth flounder Pacific Coast</t>
-  </si>
-  <si>
     <t>BGROCKPCOAST</t>
   </si>
   <si>
-    <t>Blackgill rockfish Pacific Coast</t>
-  </si>
-  <si>
     <t>BLUEROCKCAL</t>
   </si>
   <si>
-    <t>Blue rockfish California</t>
-  </si>
-  <si>
     <t>BOCACCSPCOAST</t>
   </si>
   <si>
-    <t>Bocaccio Southern Pacific Coast</t>
-  </si>
-  <si>
     <t>CABEZNCAL</t>
   </si>
   <si>
-    <t>Cabezon Northern California</t>
-  </si>
-  <si>
     <t>CABEZORECOAST</t>
   </si>
   <si>
-    <t>Cabezon Oregon Coast</t>
-  </si>
-  <si>
     <t>CABEZSCAL</t>
   </si>
   <si>
-    <t>Cabezon Southern California</t>
-  </si>
-  <si>
     <t>CALSCORPSCAL</t>
   </si>
   <si>
-    <t>California scorpionfish Southern California</t>
-  </si>
-  <si>
     <t>CHILISPCOAST</t>
   </si>
   <si>
-    <t>Chilipepper Southern Pacific Coast</t>
-  </si>
-  <si>
     <t>CMACKPCOAST</t>
   </si>
   <si>
-    <t>Pacific chub mackerel Pacific Coast</t>
-  </si>
-  <si>
     <t>COWCODSCAL</t>
   </si>
   <si>
-    <t>Cowcod Southern California</t>
-  </si>
-  <si>
     <t>CROCKPCOAST</t>
   </si>
   <si>
-    <t>Canary rockfish Pacific Coast</t>
-  </si>
-  <si>
     <t>DKROCKPCOAST</t>
   </si>
   <si>
-    <t>Darkblotched rockfish Pacific Coast</t>
-  </si>
-  <si>
     <t>DSOLEPCOAST</t>
   </si>
   <si>
-    <t>Dover sole Pacific Coast</t>
-  </si>
-  <si>
     <t>ESOLEPCOAST</t>
   </si>
   <si>
-    <t>English sole Pacific Coast</t>
-  </si>
-  <si>
     <t>GOPHERSPCOAST</t>
   </si>
   <si>
-    <t>Gopher rockfish Southern Pacific Coast</t>
-  </si>
-  <si>
     <t>GRNSTROCKPCOAST</t>
   </si>
   <si>
-    <t>Greenstriped rockfish Pacific Coast</t>
-  </si>
-  <si>
     <t>GRSPROCKNCAL</t>
   </si>
   <si>
-    <t>Greenspotted rockfish Northern Pacific Coast</t>
-  </si>
-  <si>
     <t>GRSPROCKSCAL</t>
   </si>
   <si>
-    <t>Greenspotted rockfish Southern Pacific Coast</t>
-  </si>
-  <si>
     <t>KELPGREENLINGORECOAST</t>
   </si>
   <si>
-    <t>Kelp greenling Oregon Coast</t>
-  </si>
-  <si>
     <t>LINGCODNPCOAST</t>
   </si>
   <si>
-    <t>Lingcod Northern Pacific Coast</t>
-  </si>
-  <si>
     <t>LINGCODSPCOAST</t>
   </si>
   <si>
-    <t>Lingcod Southern Pacific Coast</t>
-  </si>
-  <si>
     <t>LNOSESKAPCOAST</t>
   </si>
   <si>
-    <t>Longnose skate Pacific Coast</t>
-  </si>
-  <si>
     <t>LSTHORNHPCOAST</t>
   </si>
   <si>
-    <t>Longspine thornyhead Pacific Coast</t>
-  </si>
-  <si>
     <t>PHAKEPCOAST</t>
   </si>
   <si>
-    <t>Pacific hake Pacific Coast</t>
-  </si>
-  <si>
     <t>POPERCHPCOAST</t>
   </si>
   <si>
-    <t>Pacific ocean perch Pacific Coast</t>
-  </si>
-  <si>
     <t>PSOLEPCOAST</t>
   </si>
   <si>
-    <t>Petrale sole Pacific Coast</t>
-  </si>
-  <si>
     <t>SABLEFPCOAST</t>
   </si>
   <si>
-    <t>Sablefish Pacific Coast</t>
-  </si>
-  <si>
     <t>SBELLYROCKPCOAST</t>
   </si>
   <si>
-    <t>Shortbelly rockfish Pacific Coast</t>
-  </si>
-  <si>
     <t>SNROCKPCOAST</t>
   </si>
   <si>
-    <t>Splitnose rockfish Pacific Coast</t>
-  </si>
-  <si>
     <t>SPSDOGPCOAST</t>
   </si>
   <si>
-    <t>Spotted spiny dogfish Pacific Coast</t>
-  </si>
-  <si>
     <t>SSTHORNHPCOAST</t>
   </si>
   <si>
-    <t>Shortspine thornyhead Pacific Coast</t>
-  </si>
-  <si>
     <t>STFLOUNNPCOAST</t>
   </si>
   <si>
-    <t>Starry flounder Northern Pacific Coast</t>
-  </si>
-  <si>
     <t>STFLOUNSPCOAST</t>
   </si>
   <si>
-    <t>Starry flounder Southern Pacific Coast</t>
-  </si>
-  <si>
     <t>WROCKPCOAST</t>
   </si>
   <si>
-    <t>Widow rockfish Pacific Coast</t>
-  </si>
-  <si>
     <t>YEYEROCKPCOAST</t>
   </si>
   <si>
-    <t>Yelloweye rockfish Pacific Coast</t>
-  </si>
-  <si>
     <t>YTROCKNPCOAST</t>
   </si>
   <si>
-    <t>Yellowtail rockfish Northern Pacific Coast</t>
-  </si>
-  <si>
-    <t>Stock name</t>
-  </si>
-  <si>
     <t>Stock id</t>
   </si>
   <si>
@@ -839,6 +584,252 @@
   </si>
   <si>
     <t>Production data</t>
+  </si>
+  <si>
+    <t>Bocaccio (Sebastes paucispinis)</t>
+  </si>
+  <si>
+    <t>British Columbia Waters</t>
+  </si>
+  <si>
+    <t>Canary rockfish (Sebastes pinniger)</t>
+  </si>
+  <si>
+    <t>English sole (Parophrys vetulus)</t>
+  </si>
+  <si>
+    <t>Hecate Strait</t>
+  </si>
+  <si>
+    <t>Pacific herring (Clupea pallasii pallasii)</t>
+  </si>
+  <si>
+    <t>Central Coast</t>
+  </si>
+  <si>
+    <t>Prince Rupert District</t>
+  </si>
+  <si>
+    <t>Queen Charlotte Islands</t>
+  </si>
+  <si>
+    <t>West Coast of Vancouver Island</t>
+  </si>
+  <si>
+    <t>Pacific cod (Gadus macrocephalus)</t>
+  </si>
+  <si>
+    <t>Queen Charlotte Sound</t>
+  </si>
+  <si>
+    <t>Pacific ocean perch (Sebastes alutus)</t>
+  </si>
+  <si>
+    <t>Haida Gwaii</t>
+  </si>
+  <si>
+    <t>Rock sole (Lepidopsetta bilineata)</t>
+  </si>
+  <si>
+    <t>Sablefish (Anoplopoma fimbria)</t>
+  </si>
+  <si>
+    <t>Pacific Coast of Canada</t>
+  </si>
+  <si>
+    <t>Alaska plaice (Pleuronectes quadrituberculatus)</t>
+  </si>
+  <si>
+    <t>Bering Sea and Aleutian Islands</t>
+  </si>
+  <si>
+    <t>Arrowtooth flounder (Atheresthes stomias)</t>
+  </si>
+  <si>
+    <t>Gulf of Alaska</t>
+  </si>
+  <si>
+    <t>Atka mackerel (Pleurogrammus monopterygius)</t>
+  </si>
+  <si>
+    <t>Blue king crab (Paralithodes platypus)</t>
+  </si>
+  <si>
+    <t>Pribilof Islands</t>
+  </si>
+  <si>
+    <t>Saint Matthews Island</t>
+  </si>
+  <si>
+    <t>Dover sole (Microstomus pacificus)</t>
+  </si>
+  <si>
+    <t>Dusky rockfish (Sebastes variabilis)</t>
+  </si>
+  <si>
+    <t>Flathead sole (Hippoglossoides elassodon)</t>
+  </si>
+  <si>
+    <t>Greenland halibut (Reinhardtius hippoglossoides)</t>
+  </si>
+  <si>
+    <t>Prince William Sound</t>
+  </si>
+  <si>
+    <t>Togiak District</t>
+  </si>
+  <si>
+    <t>Northern rockfish (Sebastes polyspinis)</t>
+  </si>
+  <si>
+    <t>Northern rock sole (Lepidopsetta polyxystra)</t>
+  </si>
+  <si>
+    <t>Eastern Bering Sea and Aleutian Islands</t>
+  </si>
+  <si>
+    <t>Rex sole (Glyptocephalus zachirus)</t>
+  </si>
+  <si>
+    <t>Rougheye rockfish (Sebastes aleutianus)</t>
+  </si>
+  <si>
+    <t>Red king crab (Paralithodes camtschaticus)</t>
+  </si>
+  <si>
+    <t>Bristol Bay</t>
+  </si>
+  <si>
+    <t>Norton Sound</t>
+  </si>
+  <si>
+    <t>Eastern Bering Sea / Aleutian Islands / Gulf of Alaska</t>
+  </si>
+  <si>
+    <t>Snow crab (Chionoecetes opilio)</t>
+  </si>
+  <si>
+    <t>Bering Sea</t>
+  </si>
+  <si>
+    <t>Tanner crab (Chionoecetes bairdi)</t>
+  </si>
+  <si>
+    <t>Walleye pollock (Gadus chalcogrammus)</t>
+  </si>
+  <si>
+    <t>Aleutian Islands</t>
+  </si>
+  <si>
+    <t>Eastern Bering Sea</t>
+  </si>
+  <si>
+    <t>Yellowfin sole (Limanda aspera)</t>
+  </si>
+  <si>
+    <t>Pacific Coast</t>
+  </si>
+  <si>
+    <t>Blackgill rockfish (Sebastes melanostomus)</t>
+  </si>
+  <si>
+    <t>Blue rockfish (Sebastes mystinus)</t>
+  </si>
+  <si>
+    <t>California</t>
+  </si>
+  <si>
+    <t>Southern Pacific Coast</t>
+  </si>
+  <si>
+    <t>Cabezon (Scorpaenichthys marmoratus)</t>
+  </si>
+  <si>
+    <t>Northern California</t>
+  </si>
+  <si>
+    <t>Oregon Coast</t>
+  </si>
+  <si>
+    <t>Southern California</t>
+  </si>
+  <si>
+    <t>California scorpionfish (Scorpaena guttata)</t>
+  </si>
+  <si>
+    <t>Chilipepper (Sebastes goodei)</t>
+  </si>
+  <si>
+    <t>Pacific chub mackerel (Scomber japonicus)</t>
+  </si>
+  <si>
+    <t>Cowcod (Sebastes levis)</t>
+  </si>
+  <si>
+    <t>Darkblotched rockfish (Sebastes crameri)</t>
+  </si>
+  <si>
+    <t>Gopher rockfish (Sebastes carnatus)</t>
+  </si>
+  <si>
+    <t>Greenstriped rockfish (Sebastes elongatus)</t>
+  </si>
+  <si>
+    <t>Greenspotted rockfish (Sebastes chlorostictus)</t>
+  </si>
+  <si>
+    <t>Northern Pacific Coast</t>
+  </si>
+  <si>
+    <t>Kelp greenling (Hexagrammos decagrammus)</t>
+  </si>
+  <si>
+    <t>Lingcod (Ophiodon elongatus)</t>
+  </si>
+  <si>
+    <t>Longnose skate (Beringraja rhina)</t>
+  </si>
+  <si>
+    <t>Longspine thornyhead (Sebastolobus altivelis)</t>
+  </si>
+  <si>
+    <t>Pacific hake (Merluccius productus)</t>
+  </si>
+  <si>
+    <t>Petrale sole (Eopsetta jordani)</t>
+  </si>
+  <si>
+    <t>Shortbelly rockfish (Sebastes jordani)</t>
+  </si>
+  <si>
+    <t>Splitnose rockfish (Sebastes diploproa)</t>
+  </si>
+  <si>
+    <t>Spotted spiny dogfish (Squalus suckleyi)</t>
+  </si>
+  <si>
+    <t>Shortspine thornyhead (Sebastolobus alascanus)</t>
+  </si>
+  <si>
+    <t>Starry flounder (Platichthys stellatus)</t>
+  </si>
+  <si>
+    <t>Widow rockfish (Sebastes entomelas)</t>
+  </si>
+  <si>
+    <t>Yelloweye rockfish (Sebastes ruberrimus)</t>
+  </si>
+  <si>
+    <t>Yellowtail rockfish (Sebastes flavidus)</t>
+  </si>
+  <si>
+    <t>Species</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>WC of Vancouver Isl, Strait of Georgia, Queen Charlotte Isls</t>
   </si>
 </sst>
 </file>
@@ -1341,10 +1332,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
@@ -1700,46 +1690,46 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E88"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59D50042-0A19-C143-9CD2-57D636C7F1DF}">
+  <dimension ref="A1:F88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="I54" sqref="I54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.1640625" customWidth="1"/>
+    <col min="1" max="1" width="4.6640625" customWidth="1"/>
     <col min="2" max="2" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="83.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>172</v>
+        <v>87</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>171</v>
+        <v>267</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1747,1366 +1737,1617 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>2</v>
+        <v>188</v>
       </c>
       <c r="D3" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>189</v>
+      </c>
+      <c r="E3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>190</v>
       </c>
       <c r="D4" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+        <v>269</v>
+      </c>
+      <c r="E4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>191</v>
       </c>
       <c r="D5" t="s">
-        <v>175</v>
+        <v>192</v>
       </c>
       <c r="E5" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+      <c r="F5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>193</v>
       </c>
       <c r="D6" t="s">
-        <v>177</v>
+        <v>194</v>
       </c>
       <c r="E6" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+      <c r="F6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>193</v>
       </c>
       <c r="D7" t="s">
-        <v>177</v>
+        <v>195</v>
       </c>
       <c r="E7" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+      <c r="F7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>193</v>
       </c>
       <c r="D8" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
       <c r="E8" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+      <c r="F8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>193</v>
       </c>
       <c r="D9" t="s">
-        <v>177</v>
+        <v>197</v>
       </c>
       <c r="E9" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+      <c r="F9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>198</v>
       </c>
       <c r="D10" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+        <v>199</v>
+      </c>
+      <c r="E10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>198</v>
       </c>
       <c r="D11" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+        <v>192</v>
+      </c>
+      <c r="E11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>198</v>
       </c>
       <c r="D12" t="s">
-        <v>180</v>
+        <v>197</v>
       </c>
       <c r="E12" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+      <c r="F12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>200</v>
       </c>
       <c r="D13" t="s">
-        <v>182</v>
+        <v>201</v>
       </c>
       <c r="E13" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+      <c r="F13" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>200</v>
       </c>
       <c r="D14" t="s">
-        <v>182</v>
+        <v>197</v>
       </c>
       <c r="E14" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+      <c r="F14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>26</v>
+        <v>202</v>
       </c>
       <c r="D15" t="s">
-        <v>184</v>
+        <v>199</v>
       </c>
       <c r="E15" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+      <c r="F15" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>202</v>
       </c>
       <c r="D16" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="E16" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+      <c r="F16" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>30</v>
+        <v>203</v>
       </c>
       <c r="D17" t="s">
-        <v>187</v>
+        <v>204</v>
       </c>
       <c r="E17" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="F17" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>33</v>
+        <v>205</v>
       </c>
       <c r="D19" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+        <v>206</v>
+      </c>
+      <c r="E19" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>35</v>
+        <v>207</v>
       </c>
       <c r="D20" t="s">
-        <v>190</v>
+        <v>206</v>
       </c>
       <c r="E20" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="F20" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>3</v>
       </c>
       <c r="B21" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>37</v>
+        <v>207</v>
       </c>
       <c r="D21" t="s">
-        <v>192</v>
+        <v>208</v>
       </c>
       <c r="E21" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+      <c r="F21" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>4</v>
       </c>
       <c r="B22" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>39</v>
+        <v>209</v>
       </c>
       <c r="D22" t="s">
-        <v>193</v>
+        <v>206</v>
       </c>
       <c r="E22" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+      <c r="F22" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>5</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>41</v>
+        <v>210</v>
       </c>
       <c r="D23" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+      <c r="E23" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>6</v>
       </c>
       <c r="B24" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>43</v>
+        <v>210</v>
       </c>
       <c r="D24" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+        <v>212</v>
+      </c>
+      <c r="E24" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>7</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>45</v>
+        <v>213</v>
       </c>
       <c r="D25" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+        <v>208</v>
+      </c>
+      <c r="E25" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>8</v>
       </c>
       <c r="B26" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>47</v>
+        <v>214</v>
       </c>
       <c r="D26" t="s">
-        <v>193</v>
+        <v>208</v>
       </c>
       <c r="E26" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+      <c r="F26" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>9</v>
       </c>
       <c r="B27" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="C27" t="s">
-        <v>49</v>
+        <v>215</v>
       </c>
       <c r="D27" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+        <v>206</v>
+      </c>
+      <c r="E27" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>10</v>
       </c>
       <c r="B28" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="C28" t="s">
-        <v>51</v>
+        <v>215</v>
       </c>
       <c r="D28" t="s">
-        <v>195</v>
+        <v>208</v>
       </c>
       <c r="E28" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+      <c r="F28" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>11</v>
       </c>
       <c r="B29" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="C29" t="s">
-        <v>53</v>
+        <v>216</v>
       </c>
       <c r="D29" t="s">
-        <v>193</v>
+        <v>206</v>
       </c>
       <c r="E29" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+      <c r="F29" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>12</v>
       </c>
       <c r="B30" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="C30" t="s">
-        <v>55</v>
+        <v>193</v>
       </c>
       <c r="D30" t="s">
-        <v>199</v>
+        <v>217</v>
       </c>
       <c r="E30" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+      <c r="F30" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>13</v>
       </c>
       <c r="B31" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="C31" t="s">
-        <v>57</v>
+        <v>193</v>
       </c>
       <c r="D31" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+        <v>218</v>
+      </c>
+      <c r="E31" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>14</v>
       </c>
       <c r="B32" t="s">
-        <v>58</v>
+        <v>30</v>
       </c>
       <c r="C32" t="s">
-        <v>59</v>
+        <v>219</v>
       </c>
       <c r="D32" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="E32" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+      <c r="F32" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>15</v>
       </c>
       <c r="B33" t="s">
-        <v>60</v>
+        <v>31</v>
       </c>
       <c r="C33" t="s">
-        <v>61</v>
+        <v>219</v>
       </c>
       <c r="D33" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="E33" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+      <c r="F33" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>16</v>
       </c>
       <c r="B34" t="s">
-        <v>62</v>
+        <v>32</v>
       </c>
       <c r="C34" t="s">
-        <v>63</v>
+        <v>220</v>
       </c>
       <c r="D34" t="s">
-        <v>204</v>
+        <v>221</v>
       </c>
       <c r="E34" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+      <c r="F34" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>17</v>
       </c>
       <c r="B35" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="C35" t="s">
-        <v>65</v>
+        <v>198</v>
       </c>
       <c r="D35" t="s">
-        <v>193</v>
+        <v>208</v>
       </c>
       <c r="E35" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+      <c r="F35" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>18</v>
       </c>
       <c r="B36" t="s">
-        <v>66</v>
+        <v>34</v>
       </c>
       <c r="C36" t="s">
-        <v>67</v>
+        <v>200</v>
       </c>
       <c r="D36" t="s">
-        <v>206</v>
+        <v>221</v>
       </c>
       <c r="E36" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+      <c r="F36" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>19</v>
       </c>
       <c r="B37" t="s">
-        <v>68</v>
+        <v>35</v>
       </c>
       <c r="C37" t="s">
-        <v>69</v>
+        <v>200</v>
       </c>
       <c r="D37" t="s">
-        <v>192</v>
+        <v>208</v>
       </c>
       <c r="E37" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+      <c r="F37" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>20</v>
       </c>
       <c r="B38" t="s">
-        <v>70</v>
+        <v>36</v>
       </c>
       <c r="C38" t="s">
-        <v>71</v>
+        <v>222</v>
       </c>
       <c r="D38" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E38" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+        <v>124</v>
+      </c>
+      <c r="F38" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>21</v>
       </c>
       <c r="B39" t="s">
-        <v>72</v>
+        <v>37</v>
       </c>
       <c r="C39" t="s">
-        <v>73</v>
+        <v>223</v>
       </c>
       <c r="D39" t="s">
-        <v>193</v>
+        <v>206</v>
       </c>
       <c r="E39" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+      <c r="F39" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>22</v>
       </c>
       <c r="B40" t="s">
-        <v>74</v>
+        <v>38</v>
       </c>
       <c r="C40" t="s">
-        <v>75</v>
+        <v>223</v>
       </c>
       <c r="D40" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+        <v>208</v>
+      </c>
+      <c r="E40" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>23</v>
       </c>
       <c r="B41" t="s">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="C41" t="s">
-        <v>77</v>
+        <v>224</v>
       </c>
       <c r="D41" t="s">
-        <v>204</v>
+        <v>225</v>
       </c>
       <c r="E41" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+      <c r="F41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>24</v>
       </c>
       <c r="B42" t="s">
-        <v>78</v>
+        <v>40</v>
       </c>
       <c r="C42" t="s">
-        <v>79</v>
+        <v>224</v>
       </c>
       <c r="D42" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+        <v>226</v>
+      </c>
+      <c r="E42" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>25</v>
       </c>
       <c r="B43" t="s">
-        <v>80</v>
+        <v>41</v>
       </c>
       <c r="C43" t="s">
-        <v>81</v>
+        <v>224</v>
       </c>
       <c r="D43" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+      <c r="E43" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>26</v>
       </c>
       <c r="B44" t="s">
-        <v>82</v>
+        <v>42</v>
       </c>
       <c r="C44" t="s">
-        <v>83</v>
+        <v>203</v>
       </c>
       <c r="D44" t="s">
-        <v>198</v>
+        <v>227</v>
       </c>
       <c r="E44" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+        <v>113</v>
+      </c>
+      <c r="F44" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>27</v>
       </c>
       <c r="B45" t="s">
-        <v>84</v>
+        <v>43</v>
       </c>
       <c r="C45" t="s">
-        <v>85</v>
+        <v>228</v>
       </c>
       <c r="D45" t="s">
-        <v>215</v>
+        <v>229</v>
       </c>
       <c r="E45" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+      <c r="F45" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>28</v>
       </c>
       <c r="B46" t="s">
-        <v>86</v>
+        <v>44</v>
       </c>
       <c r="C46" t="s">
-        <v>87</v>
+        <v>230</v>
       </c>
       <c r="D46" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="E46" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+        <v>132</v>
+      </c>
+      <c r="F46" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>29</v>
       </c>
       <c r="B47" t="s">
-        <v>88</v>
+        <v>45</v>
       </c>
       <c r="C47" t="s">
-        <v>89</v>
+        <v>231</v>
       </c>
       <c r="D47" t="s">
-        <v>195</v>
+        <v>232</v>
       </c>
       <c r="E47" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+      <c r="F47" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>30</v>
       </c>
       <c r="B48" t="s">
-        <v>90</v>
+        <v>46</v>
       </c>
       <c r="C48" t="s">
-        <v>91</v>
+        <v>231</v>
       </c>
       <c r="D48" t="s">
-        <v>215</v>
+        <v>233</v>
       </c>
       <c r="E48" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+      <c r="F48" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>31</v>
       </c>
       <c r="B49" t="s">
-        <v>92</v>
+        <v>47</v>
       </c>
       <c r="C49" t="s">
-        <v>93</v>
+        <v>231</v>
       </c>
       <c r="D49" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="E49" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+      <c r="F49" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>32</v>
       </c>
       <c r="B50" t="s">
-        <v>94</v>
+        <v>48</v>
       </c>
       <c r="C50" t="s">
-        <v>95</v>
+        <v>234</v>
       </c>
       <c r="D50" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+        <v>206</v>
+      </c>
+      <c r="E50" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>1</v>
       </c>
       <c r="B52" t="s">
-        <v>97</v>
+        <v>50</v>
       </c>
       <c r="C52" t="s">
-        <v>98</v>
+        <v>207</v>
       </c>
       <c r="D52" t="s">
-        <v>222</v>
+        <v>235</v>
       </c>
       <c r="E52" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+      <c r="F52" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>2</v>
       </c>
       <c r="B53" t="s">
-        <v>99</v>
+        <v>51</v>
       </c>
       <c r="C53" t="s">
-        <v>100</v>
+        <v>236</v>
       </c>
       <c r="D53" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+        <v>235</v>
+      </c>
+      <c r="E53" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>3</v>
       </c>
       <c r="B54" t="s">
-        <v>101</v>
+        <v>52</v>
       </c>
       <c r="C54" t="s">
-        <v>102</v>
+        <v>237</v>
       </c>
       <c r="D54" t="s">
-        <v>224</v>
+        <v>238</v>
       </c>
       <c r="E54" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+        <v>139</v>
+      </c>
+      <c r="F54" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>4</v>
       </c>
       <c r="B55" t="s">
-        <v>103</v>
+        <v>53</v>
       </c>
       <c r="C55" t="s">
-        <v>104</v>
+        <v>188</v>
       </c>
       <c r="D55" t="s">
-        <v>226</v>
+        <v>239</v>
       </c>
       <c r="E55" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+        <v>141</v>
+      </c>
+      <c r="F55" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>5</v>
       </c>
       <c r="B56" t="s">
-        <v>105</v>
+        <v>54</v>
       </c>
       <c r="C56" t="s">
-        <v>106</v>
+        <v>240</v>
       </c>
       <c r="D56" t="s">
-        <v>228</v>
+        <v>241</v>
       </c>
       <c r="E56" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+        <v>143</v>
+      </c>
+      <c r="F56" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>6</v>
       </c>
       <c r="B57" t="s">
-        <v>107</v>
+        <v>55</v>
       </c>
       <c r="C57" t="s">
-        <v>108</v>
+        <v>240</v>
       </c>
       <c r="D57" t="s">
-        <v>230</v>
+        <v>242</v>
       </c>
       <c r="E57" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+      <c r="F57" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>7</v>
       </c>
       <c r="B58" t="s">
-        <v>109</v>
+        <v>56</v>
       </c>
       <c r="C58" t="s">
-        <v>110</v>
+        <v>240</v>
       </c>
       <c r="D58" t="s">
-        <v>232</v>
+        <v>243</v>
       </c>
       <c r="E58" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+        <v>147</v>
+      </c>
+      <c r="F58" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>8</v>
       </c>
       <c r="B59" t="s">
-        <v>111</v>
+        <v>57</v>
       </c>
       <c r="C59" t="s">
-        <v>112</v>
+        <v>244</v>
       </c>
       <c r="D59" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+        <v>243</v>
+      </c>
+      <c r="E59" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>9</v>
       </c>
       <c r="B60" t="s">
-        <v>113</v>
+        <v>58</v>
       </c>
       <c r="C60" t="s">
-        <v>114</v>
+        <v>245</v>
       </c>
       <c r="D60" t="s">
-        <v>217</v>
+        <v>239</v>
       </c>
       <c r="E60" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+        <v>132</v>
+      </c>
+      <c r="F60" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>10</v>
       </c>
       <c r="B61" t="s">
-        <v>115</v>
+        <v>59</v>
       </c>
       <c r="C61" t="s">
-        <v>116</v>
+        <v>246</v>
       </c>
       <c r="D61" t="s">
         <v>235</v>
       </c>
       <c r="E61" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+      <c r="F61" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>11</v>
       </c>
       <c r="B62" t="s">
-        <v>117</v>
+        <v>60</v>
       </c>
       <c r="C62" t="s">
-        <v>118</v>
+        <v>247</v>
       </c>
       <c r="D62" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+        <v>243</v>
+      </c>
+      <c r="E62" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>12</v>
       </c>
       <c r="B63" t="s">
-        <v>119</v>
+        <v>61</v>
       </c>
       <c r="C63" t="s">
-        <v>120</v>
+        <v>190</v>
       </c>
       <c r="D63" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="E63" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+        <v>153</v>
+      </c>
+      <c r="F63" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>13</v>
       </c>
       <c r="B64" t="s">
-        <v>121</v>
+        <v>62</v>
       </c>
       <c r="C64" t="s">
-        <v>122</v>
+        <v>248</v>
       </c>
       <c r="D64" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="E64" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+      <c r="F64" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>14</v>
       </c>
       <c r="B65" t="s">
-        <v>123</v>
+        <v>63</v>
       </c>
       <c r="C65" t="s">
-        <v>124</v>
+        <v>213</v>
       </c>
       <c r="D65" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="E65" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+        <v>157</v>
+      </c>
+      <c r="F65" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>15</v>
       </c>
       <c r="B66" t="s">
-        <v>125</v>
+        <v>64</v>
       </c>
       <c r="C66" t="s">
-        <v>126</v>
+        <v>191</v>
       </c>
       <c r="D66" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="E66" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+        <v>159</v>
+      </c>
+      <c r="F66" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>16</v>
       </c>
       <c r="B67" t="s">
-        <v>127</v>
+        <v>65</v>
       </c>
       <c r="C67" t="s">
-        <v>128</v>
+        <v>249</v>
       </c>
       <c r="D67" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="E67" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="F67" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>17</v>
       </c>
       <c r="B68" t="s">
-        <v>129</v>
+        <v>66</v>
       </c>
       <c r="C68" t="s">
-        <v>130</v>
+        <v>250</v>
       </c>
       <c r="D68" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="E68" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+        <v>147</v>
+      </c>
+      <c r="F68" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>18</v>
       </c>
       <c r="B69" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="C69" t="s">
-        <v>132</v>
+        <v>251</v>
       </c>
       <c r="D69" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+      <c r="E69" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>19</v>
       </c>
       <c r="B70" t="s">
-        <v>133</v>
+        <v>68</v>
       </c>
       <c r="C70" t="s">
-        <v>134</v>
+        <v>251</v>
       </c>
       <c r="D70" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+        <v>239</v>
+      </c>
+      <c r="E70" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>20</v>
       </c>
       <c r="B71" t="s">
-        <v>135</v>
+        <v>69</v>
       </c>
       <c r="C71" t="s">
-        <v>136</v>
+        <v>253</v>
       </c>
       <c r="D71" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="E71" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+        <v>163</v>
+      </c>
+      <c r="F71" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>21</v>
       </c>
       <c r="B72" t="s">
-        <v>137</v>
+        <v>70</v>
       </c>
       <c r="C72" t="s">
-        <v>138</v>
+        <v>254</v>
       </c>
       <c r="D72" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="E72" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+        <v>164</v>
+      </c>
+      <c r="F72" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>22</v>
       </c>
       <c r="B73" t="s">
-        <v>139</v>
+        <v>71</v>
       </c>
       <c r="C73" t="s">
-        <v>140</v>
+        <v>254</v>
       </c>
       <c r="D73" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
       <c r="E73" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+      <c r="F73" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>23</v>
       </c>
       <c r="B74" t="s">
-        <v>141</v>
+        <v>72</v>
       </c>
       <c r="C74" t="s">
-        <v>142</v>
+        <v>255</v>
       </c>
       <c r="D74" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+        <v>235</v>
+      </c>
+      <c r="E74" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>24</v>
       </c>
       <c r="B75" t="s">
-        <v>143</v>
+        <v>73</v>
       </c>
       <c r="C75" t="s">
-        <v>144</v>
+        <v>256</v>
       </c>
       <c r="D75" t="s">
-        <v>253</v>
+        <v>235</v>
       </c>
       <c r="E75" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+        <v>168</v>
+      </c>
+      <c r="F75" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>25</v>
       </c>
       <c r="B76" t="s">
-        <v>145</v>
+        <v>74</v>
       </c>
       <c r="C76" t="s">
-        <v>146</v>
+        <v>257</v>
       </c>
       <c r="D76" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="E76" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+      <c r="F76" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>26</v>
       </c>
       <c r="B77" t="s">
-        <v>147</v>
+        <v>75</v>
       </c>
       <c r="C77" t="s">
-        <v>148</v>
+        <v>200</v>
       </c>
       <c r="D77" t="s">
-        <v>256</v>
+        <v>235</v>
       </c>
       <c r="E77" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+        <v>171</v>
+      </c>
+      <c r="F77" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>27</v>
       </c>
       <c r="B78" t="s">
-        <v>149</v>
+        <v>76</v>
       </c>
       <c r="C78" t="s">
-        <v>150</v>
+        <v>258</v>
       </c>
       <c r="D78" t="s">
-        <v>257</v>
+        <v>235</v>
       </c>
       <c r="E78" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+        <v>172</v>
+      </c>
+      <c r="F78" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>28</v>
       </c>
       <c r="B79" t="s">
-        <v>151</v>
+        <v>77</v>
       </c>
       <c r="C79" t="s">
-        <v>152</v>
+        <v>203</v>
       </c>
       <c r="D79" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+        <v>235</v>
+      </c>
+      <c r="E79" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>29</v>
       </c>
       <c r="B80" t="s">
-        <v>153</v>
+        <v>78</v>
       </c>
       <c r="C80" t="s">
-        <v>154</v>
+        <v>259</v>
       </c>
       <c r="D80" t="s">
-        <v>259</v>
+        <v>235</v>
       </c>
       <c r="E80" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+        <v>174</v>
+      </c>
+      <c r="F80" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>30</v>
       </c>
       <c r="B81" t="s">
-        <v>155</v>
+        <v>79</v>
       </c>
       <c r="C81" t="s">
-        <v>156</v>
+        <v>260</v>
       </c>
       <c r="D81" t="s">
-        <v>249</v>
+        <v>235</v>
       </c>
       <c r="E81" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+        <v>164</v>
+      </c>
+      <c r="F81" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>31</v>
       </c>
       <c r="B82" t="s">
-        <v>157</v>
+        <v>80</v>
       </c>
       <c r="C82" t="s">
-        <v>158</v>
+        <v>261</v>
       </c>
       <c r="D82" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+        <v>235</v>
+      </c>
+      <c r="E82" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>32</v>
       </c>
       <c r="B83" t="s">
-        <v>159</v>
+        <v>81</v>
       </c>
       <c r="C83" t="s">
-        <v>160</v>
+        <v>262</v>
       </c>
       <c r="D83" t="s">
-        <v>262</v>
+        <v>235</v>
       </c>
       <c r="E83" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+        <v>177</v>
+      </c>
+      <c r="F83" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>33</v>
       </c>
       <c r="B84" t="s">
-        <v>161</v>
+        <v>82</v>
       </c>
       <c r="C84" t="s">
-        <v>162</v>
+        <v>263</v>
       </c>
       <c r="D84" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
       <c r="E84" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+        <v>179</v>
+      </c>
+      <c r="F84" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>34</v>
       </c>
       <c r="B85" t="s">
-        <v>163</v>
+        <v>83</v>
       </c>
       <c r="C85" t="s">
-        <v>164</v>
-      </c>
-      <c r="E85" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+        <v>263</v>
+      </c>
+      <c r="D85" t="s">
+        <v>239</v>
+      </c>
+      <c r="F85" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>35</v>
       </c>
       <c r="B86" t="s">
-        <v>165</v>
+        <v>84</v>
       </c>
       <c r="C86" t="s">
-        <v>166</v>
+        <v>264</v>
       </c>
       <c r="D86" t="s">
-        <v>267</v>
+        <v>235</v>
       </c>
       <c r="E86" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+        <v>182</v>
+      </c>
+      <c r="F86" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>36</v>
       </c>
       <c r="B87" t="s">
-        <v>167</v>
+        <v>85</v>
       </c>
       <c r="C87" t="s">
-        <v>168</v>
+        <v>265</v>
       </c>
       <c r="D87" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+        <v>235</v>
+      </c>
+      <c r="E87" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>37</v>
       </c>
       <c r="B88" t="s">
-        <v>169</v>
+        <v>86</v>
       </c>
       <c r="C88" t="s">
-        <v>170</v>
+        <v>266</v>
       </c>
       <c r="D88" t="s">
-        <v>270</v>
+        <v>252</v>
       </c>
       <c r="E88" t="s">
-        <v>270</v>
+        <v>185</v>
+      </c>
+      <c r="F88" t="s">
+        <v>185</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>